<commit_message>
Cambiar etiqueta de horario no existente
Co-Authored-By: Juan Diego <68799845+juandiego-gm@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple (22).xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple (22).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A38F6A5-2162-2B42-994D-746A45B9E21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F21978-1FED-A34E-8ACB-922A262258B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="42">
   <si>
     <t>EMPLEADO</t>
   </si>
@@ -143,6 +143,9 @@
   </si>
   <si>
     <t>OFICINA,DEFAULT-LIBRE</t>
+  </si>
+  <si>
+    <t>OFICINA2</t>
   </si>
 </sst>
 </file>
@@ -529,8 +532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -855,7 +858,7 @@
         <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
Añadir tratamientos de errores a la revisión de la plantilla de planificación horaria
Co-Authored-By: Juan Diego <68799845+juandiego-gm@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/servidor/leerPlantillas/plantillaPlanificacionMultiple (22).xlsx
+++ b/servidor/leerPlantillas/plantillaPlanificacionMultiple (22).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/casapazmino/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F21978-1FED-A34E-8ACB-922A262258B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEE881FF-36BA-CE49-B180-0E7A99D1AA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33600" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificacion" sheetId="1" r:id="rId1"/>
@@ -533,7 +533,7 @@
   <dimension ref="A1:AG5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="C1" sqref="C1:AG1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>